<commit_message>
updated data, transitions, dropdown
</commit_message>
<xml_diff>
--- a/Cost of a night out around the world.xlsx
+++ b/Cost of a night out around the world.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\em\Documents\MakeoverMonday\Datasets\2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tuckergordon/Desktop/Makeover Monday/NightOut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04ECDB89-22F3-4F0C-B0A1-C83CBC83A24D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A90186-4F30-E444-A66C-61216E75C29D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30760" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$A$92</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -153,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,22 +477,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -523,7 +527,7 @@
         <v>69.38</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -540,7 +544,7 @@
         <v>21.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -557,7 +561,7 @@
         <v>11.87</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -574,7 +578,7 @@
         <v>10.92</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -591,7 +595,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -608,7 +612,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -625,7 +629,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -642,7 +646,7 @@
         <v>75.42</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -659,7 +663,7 @@
         <v>24.64</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -676,7 +680,7 @@
         <v>13.57</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -693,7 +697,7 @@
         <v>6.32</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -710,7 +714,7 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -727,7 +731,7 @@
         <v>25.55</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -744,7 +748,7 @@
         <v>27.59</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -761,7 +765,7 @@
         <v>55.51</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -778,7 +782,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -795,7 +799,7 @@
         <v>4.21</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -812,7 +816,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -829,7 +833,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -846,7 +850,7 @@
         <v>3.22</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -863,7 +867,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -880,7 +884,7 @@
         <v>93.48</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -897,7 +901,7 @@
         <v>42.12</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -914,7 +918,7 @@
         <v>12.41</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -931,7 +935,7 @@
         <v>10.37</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -948,7 +952,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -965,7 +969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -982,7 +986,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -999,7 +1003,7 @@
         <v>57.26</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1016,7 +1020,7 @@
         <v>43.93</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1033,7 +1037,7 @@
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1050,7 +1054,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1071,7 @@
         <v>2.29</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1084,7 +1088,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1101,7 +1105,7 @@
         <v>15.83</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>144.03</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1135,7 +1139,7 @@
         <v>38.450000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1152,7 +1156,7 @@
         <v>16.329999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>16.53</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1190,7 @@
         <v>5.09</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1203,7 +1207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1224,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1237,7 +1241,7 @@
         <v>85.11</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>40.090000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1271,7 +1275,7 @@
         <v>13.15</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1288,7 +1292,7 @@
         <v>11.06</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -1305,7 +1309,7 @@
         <v>5.37</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1322,7 +1326,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1356,7 +1360,7 @@
         <v>53.46</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1373,7 +1377,7 @@
         <v>23.63</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1390,7 +1394,7 @@
         <v>9.43</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -1407,7 +1411,7 @@
         <v>8.6300000000000008</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -1441,7 +1445,7 @@
         <v>19.440000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -1458,7 +1462,7 @@
         <v>14.48</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1475,7 +1479,7 @@
         <v>57.02</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +1496,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>8.48</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -1526,7 +1530,7 @@
         <v>5.21</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -1543,7 +1547,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -1560,7 +1564,7 @@
         <v>14.76</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -1577,7 +1581,7 @@
         <v>18.489999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1594,7 +1598,7 @@
         <v>111.04</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>58.6</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -1628,7 +1632,7 @@
         <v>16.190000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -1645,7 +1649,7 @@
         <v>19.91</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -1662,7 +1666,7 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -1679,7 +1683,7 @@
         <v>27.14</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1713,7 +1717,7 @@
         <v>78.62</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1730,7 +1734,7 @@
         <v>34.590000000000003</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1751,7 @@
         <v>13.96</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -1764,7 +1768,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>4.42</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -1798,7 +1802,7 @@
         <v>19.66</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -1815,7 +1819,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>121.26</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -1849,7 +1853,7 @@
         <v>62.18</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -1866,7 +1870,7 @@
         <v>16.73</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>17.02</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -1900,7 +1904,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -1917,7 +1921,7 @@
         <v>18.579999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -1934,7 +1938,7 @@
         <v>18.940000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -1951,7 +1955,7 @@
         <v>106.51</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>52.99</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -1985,7 +1989,7 @@
         <v>19.61</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -2002,7 +2006,7 @@
         <v>24.38</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -2019,7 +2023,7 @@
         <v>6.89</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -2036,7 +2040,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -2054,6 +2058,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A92" xr:uid="{B521B1B8-73DC-A44E-BA93-E44796E97E3E}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Party night"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>